<commit_message>
Update Gem Mine Strategy Template.xlsx
</commit_message>
<xml_diff>
--- a/Workbooks/Gem Mine Strategy Template.xlsx
+++ b/Workbooks/Gem Mine Strategy Template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\wide_\Documents\GitHub\Token-Jenny-Public\Workbooks\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3155A991-D291-43FE-A016-755A4CB3FFBD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C30BC59A-FC4A-4C94-AA7C-A0FE7AC3FD4E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="15796" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="56">
   <si>
     <t>JENN</t>
   </si>
@@ -95,15 +95,6 @@
     <t>Registration Cutoff At</t>
   </si>
   <si>
-    <t>HTTP URL HERE</t>
-  </si>
-  <si>
-    <t>TJ Registration Cutoff Runway</t>
-  </si>
-  <si>
-    <t>TJ Fee Cut</t>
-  </si>
-  <si>
     <t>The numbers below are estimates.  The blockends truly calculates based on the wallets registration block and those will unpredictably vary.                                                                              Also due to rounding, there is a possibility that there is "mine dust" left over following the blockends.  This is withdrawable assuming all miners have claimed.</t>
   </si>
   <si>
@@ -201,6 +192,18 @@
   </si>
   <si>
     <t>Amethyst</t>
+  </si>
+  <si>
+    <t>Registration Cutoff Runway</t>
+  </si>
+  <si>
+    <t>https://bit.ly/2ShMFZj</t>
+  </si>
+  <si>
+    <t>https://bit.ly/3gYifn0</t>
+  </si>
+  <si>
+    <t>TJ Fee Percentage</t>
   </si>
 </sst>
 </file>
@@ -210,7 +213,7 @@
   <numFmts count="1">
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -248,6 +251,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -272,12 +283,13 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="3">
+  <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="44" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -293,63 +305,68 @@
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="37" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="3" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="3" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="37" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="37" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="37" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="3">
+  <cellStyles count="4">
     <cellStyle name="Currency" xfId="1" builtinId="4"/>
+    <cellStyle name="Hyperlink" xfId="3" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Percent" xfId="2" builtinId="5"/>
   </cellStyles>
@@ -720,8 +737,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B10:J45"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="I31" sqref="I31"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I15" sqref="I15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -749,38 +766,38 @@
       <c r="J10" s="5"/>
     </row>
     <row r="11" spans="2:10" ht="14.35" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B11" s="14" t="str">
+      <c r="B11" s="15" t="str">
         <f>"Gem Mine Planner for "&amp;C16&amp;" status as "&amp;INDEX('Dropdown Data'!C3:C7, MATCH(C22, 'Dropdown Data'!B3:B7, 0))</f>
         <v>Gem Mine Planner for JENN status as Diamond</v>
       </c>
-      <c r="C11" s="14"/>
-      <c r="D11" s="14"/>
-      <c r="E11" s="14"/>
-      <c r="F11" s="14"/>
-      <c r="G11" s="14"/>
-      <c r="H11" s="14"/>
+      <c r="C11" s="15"/>
+      <c r="D11" s="15"/>
+      <c r="E11" s="15"/>
+      <c r="F11" s="15"/>
+      <c r="G11" s="15"/>
+      <c r="H11" s="15"/>
       <c r="I11" s="5"/>
       <c r="J11" s="5"/>
     </row>
     <row r="12" spans="2:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B12" s="14"/>
-      <c r="C12" s="14"/>
-      <c r="D12" s="14"/>
-      <c r="E12" s="14"/>
-      <c r="F12" s="14"/>
-      <c r="G12" s="14"/>
-      <c r="H12" s="14"/>
+      <c r="B12" s="15"/>
+      <c r="C12" s="15"/>
+      <c r="D12" s="15"/>
+      <c r="E12" s="15"/>
+      <c r="F12" s="15"/>
+      <c r="G12" s="15"/>
+      <c r="H12" s="15"/>
       <c r="I12" s="5"/>
       <c r="J12" s="5"/>
     </row>
     <row r="13" spans="2:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B13" s="14"/>
-      <c r="C13" s="14"/>
-      <c r="D13" s="14"/>
-      <c r="E13" s="14"/>
-      <c r="F13" s="14"/>
-      <c r="G13" s="14"/>
-      <c r="H13" s="14"/>
+      <c r="B13" s="15"/>
+      <c r="C13" s="15"/>
+      <c r="D13" s="15"/>
+      <c r="E13" s="15"/>
+      <c r="F13" s="15"/>
+      <c r="G13" s="15"/>
+      <c r="H13" s="15"/>
       <c r="I13" s="5"/>
       <c r="J13" s="5"/>
     </row>
@@ -796,174 +813,174 @@
       <c r="B15" t="s">
         <v>1</v>
       </c>
-      <c r="C15" s="19" t="s">
+      <c r="C15" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="E15" s="10" t="s">
-        <v>21</v>
-      </c>
-      <c r="F15" s="10"/>
-      <c r="G15" s="17">
+      <c r="E15" s="16" t="s">
+        <v>55</v>
+      </c>
+      <c r="F15" s="16"/>
+      <c r="G15" s="19">
         <f>INDEX('Dropdown Data'!G3:G7, MATCH(C22, 'Dropdown Data'!B3:B7, 0))</f>
         <v>0.5</v>
       </c>
-      <c r="H15" s="17"/>
+      <c r="H15" s="19"/>
     </row>
     <row r="16" spans="2:10" x14ac:dyDescent="0.45">
       <c r="B16" t="s">
         <v>2</v>
       </c>
-      <c r="C16" s="19" t="s">
+      <c r="C16" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="E16" s="10" t="s">
+      <c r="E16" s="16" t="s">
         <v>6</v>
       </c>
-      <c r="F16" s="10"/>
-      <c r="G16" s="21">
+      <c r="F16" s="16"/>
+      <c r="G16" s="17">
         <v>1200000</v>
       </c>
-      <c r="H16" s="21"/>
+      <c r="H16" s="17"/>
     </row>
     <row r="17" spans="2:8" x14ac:dyDescent="0.45">
       <c r="B17" t="s">
         <v>3</v>
       </c>
-      <c r="C17" s="19">
+      <c r="C17" s="11">
         <v>18</v>
       </c>
-      <c r="E17" s="10" t="s">
+      <c r="E17" s="16" t="s">
         <v>7</v>
       </c>
-      <c r="F17" s="10"/>
-      <c r="G17" s="22">
+      <c r="F17" s="16"/>
+      <c r="G17" s="24">
         <v>14765000</v>
       </c>
-      <c r="H17" s="22"/>
+      <c r="H17" s="24"/>
     </row>
     <row r="18" spans="2:8" x14ac:dyDescent="0.45">
       <c r="B18" t="s">
         <v>4</v>
       </c>
-      <c r="C18" s="20">
+      <c r="C18" s="12">
         <v>8999999</v>
       </c>
-      <c r="E18" s="10" t="s">
+      <c r="E18" s="16" t="s">
         <v>8</v>
       </c>
-      <c r="F18" s="10"/>
-      <c r="G18" s="22">
+      <c r="F18" s="16"/>
+      <c r="G18" s="24">
         <v>2.0000000000000001E-4</v>
       </c>
-      <c r="H18" s="22"/>
+      <c r="H18" s="24"/>
     </row>
     <row r="19" spans="2:8" x14ac:dyDescent="0.45">
       <c r="B19" t="s">
         <v>5</v>
       </c>
-      <c r="C19" s="20">
+      <c r="C19" s="12">
         <v>599999</v>
       </c>
-      <c r="E19" s="10" t="s">
+      <c r="E19" s="16" t="s">
         <v>14</v>
       </c>
-      <c r="F19" s="10"/>
-      <c r="G19" s="9">
+      <c r="F19" s="16"/>
+      <c r="G19" s="18">
         <f>ROUNDUP((C18/G16)*INDEX('Dropdown Data'!F3:F7, MATCH(C22, 'Dropdown Data'!B3:B7, 0)), 0)</f>
         <v>383</v>
       </c>
-      <c r="H19" s="9"/>
+      <c r="H19" s="18"/>
     </row>
     <row r="20" spans="2:8" x14ac:dyDescent="0.45">
       <c r="B20" t="s">
         <v>15</v>
       </c>
-      <c r="C20" s="19" t="s">
-        <v>19</v>
-      </c>
-      <c r="E20" s="10" t="str">
+      <c r="C20" s="14" t="s">
+        <v>53</v>
+      </c>
+      <c r="E20" s="16" t="str">
         <f>"Minimum Entry Free ("&amp;INDEX('Dropdown Data'!E3:E7, MATCH(C22, 'Dropdown Data'!B3:B7, 0))&amp;")"</f>
         <v>Minimum Entry Free (JENN/ONE LP)</v>
       </c>
-      <c r="F20" s="10"/>
-      <c r="G20" s="8">
+      <c r="F20" s="16"/>
+      <c r="G20" s="21">
         <f>INDEX('Dropdown Data'!D3:D7, MATCH(C22, 'Dropdown Data'!B3:B7, 0))</f>
         <v>50</v>
       </c>
-      <c r="H20" s="8"/>
+      <c r="H20" s="21"/>
     </row>
     <row r="21" spans="2:8" x14ac:dyDescent="0.45">
       <c r="B21" t="s">
         <v>16</v>
       </c>
-      <c r="C21" s="19" t="s">
-        <v>19</v>
-      </c>
-      <c r="E21" s="10" t="str">
+      <c r="C21" s="14" t="s">
+        <v>54</v>
+      </c>
+      <c r="E21" s="16" t="str">
         <f>"Set Mine Fee ("&amp;INDEX('Dropdown Data'!E3:E7, MATCH(C22, 'Dropdown Data'!B3:B7, 0))&amp;")"</f>
         <v>Set Mine Fee (JENN/ONE LP)</v>
       </c>
-      <c r="F21" s="10"/>
-      <c r="G21" s="21">
+      <c r="F21" s="16"/>
+      <c r="G21" s="17">
         <v>175</v>
       </c>
-      <c r="H21" s="21"/>
+      <c r="H21" s="17"/>
     </row>
     <row r="22" spans="2:8" x14ac:dyDescent="0.45">
       <c r="B22" t="s">
-        <v>25</v>
-      </c>
-      <c r="C22" s="19" t="s">
-        <v>26</v>
-      </c>
-      <c r="E22" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="C22" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="E22" s="16" t="s">
         <v>17</v>
       </c>
-      <c r="F22" s="10"/>
-      <c r="G22" s="7">
+      <c r="F22" s="16"/>
+      <c r="G22" s="22">
         <f>G21/G18</f>
         <v>875000</v>
       </c>
-      <c r="H22" s="7"/>
+      <c r="H22" s="22"/>
     </row>
     <row r="23" spans="2:8" x14ac:dyDescent="0.45">
       <c r="C23" s="4"/>
-      <c r="E23" s="10" t="s">
-        <v>20</v>
-      </c>
-      <c r="F23" s="10"/>
-      <c r="G23" s="15">
+      <c r="E23" s="16" t="s">
+        <v>52</v>
+      </c>
+      <c r="F23" s="16"/>
+      <c r="G23" s="23">
         <f>G22*0.25</f>
         <v>218750</v>
       </c>
-      <c r="H23" s="15"/>
+      <c r="H23" s="23"/>
     </row>
     <row r="24" spans="2:8" x14ac:dyDescent="0.45">
       <c r="C24" s="4"/>
-      <c r="E24" s="13"/>
-      <c r="F24" s="13"/>
-      <c r="G24" s="16"/>
-      <c r="H24" s="16"/>
+      <c r="E24" s="8"/>
+      <c r="F24" s="8"/>
+      <c r="G24" s="9"/>
+      <c r="H24" s="9"/>
     </row>
     <row r="25" spans="2:8" x14ac:dyDescent="0.45">
-      <c r="B25" s="24" t="s">
-        <v>22</v>
-      </c>
-      <c r="C25" s="24"/>
-      <c r="D25" s="24"/>
-      <c r="E25" s="24"/>
-      <c r="F25" s="24"/>
-      <c r="G25" s="24"/>
-      <c r="H25" s="24"/>
+      <c r="B25" s="20" t="s">
+        <v>19</v>
+      </c>
+      <c r="C25" s="20"/>
+      <c r="D25" s="20"/>
+      <c r="E25" s="20"/>
+      <c r="F25" s="20"/>
+      <c r="G25" s="20"/>
+      <c r="H25" s="20"/>
     </row>
     <row r="26" spans="2:8" x14ac:dyDescent="0.45">
-      <c r="B26" s="24"/>
-      <c r="C26" s="24"/>
-      <c r="D26" s="24"/>
-      <c r="E26" s="24"/>
-      <c r="F26" s="24"/>
-      <c r="G26" s="24"/>
-      <c r="H26" s="24"/>
+      <c r="B26" s="20"/>
+      <c r="C26" s="20"/>
+      <c r="D26" s="20"/>
+      <c r="E26" s="20"/>
+      <c r="F26" s="20"/>
+      <c r="G26" s="20"/>
+      <c r="H26" s="20"/>
     </row>
     <row r="27" spans="2:8" ht="42.75" x14ac:dyDescent="0.45">
       <c r="B27" s="2" t="s">
@@ -972,42 +989,42 @@
       <c r="C27" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="D27" s="11" t="s">
+      <c r="D27" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="E27" s="11" t="s">
+      <c r="E27" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="F27" s="11" t="s">
-        <v>23</v>
+      <c r="F27" s="7" t="s">
+        <v>20</v>
       </c>
       <c r="G27" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="H27" s="11" t="s">
-        <v>24</v>
+      <c r="H27" s="7" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="28" spans="2:8" x14ac:dyDescent="0.45">
-      <c r="B28" s="18"/>
+      <c r="B28" s="10"/>
       <c r="C28" s="6">
         <f>IFERROR($G$17+($G$16/(B28*$G$18)), 0)</f>
         <v>0</v>
       </c>
       <c r="D28" s="4">
-        <f>B28*$G$18</f>
+        <f t="shared" ref="D28:D45" si="0">B28*$G$18</f>
         <v>0</v>
       </c>
       <c r="E28" s="6">
-        <f>C28-$G$23</f>
+        <f t="shared" ref="E28:E45" si="1">C28-$G$23</f>
         <v>-218750</v>
       </c>
       <c r="F28" s="6">
-        <f>B28*($G$21*(1-$G$15))</f>
+        <f t="shared" ref="F28:F45" si="2">B28*($G$21*(1-$G$15))</f>
         <v>0</v>
       </c>
       <c r="G28" s="6">
-        <f>C28-$G$16</f>
+        <f t="shared" ref="G28:G45" si="3">C28-$G$16</f>
         <v>-1200000</v>
       </c>
       <c r="H28" s="4">
@@ -1020,23 +1037,23 @@
         <v>100</v>
       </c>
       <c r="C29" s="6">
-        <f>$G$17+($G$16/(B29*$G$18))</f>
+        <f t="shared" ref="C29:C45" si="4">$G$17+($G$16/(B29*$G$18))</f>
         <v>74765000</v>
       </c>
       <c r="D29" s="4">
-        <f>B29*$G$18</f>
+        <f t="shared" si="0"/>
         <v>0.02</v>
       </c>
       <c r="E29" s="6">
-        <f>C29-$G$23</f>
+        <f t="shared" si="1"/>
         <v>74546250</v>
       </c>
       <c r="F29" s="6">
-        <f>B29*($G$21*(1-$G$15))</f>
+        <f t="shared" si="2"/>
         <v>8750</v>
       </c>
       <c r="G29" s="6">
-        <f>C29-$G$16</f>
+        <f t="shared" si="3"/>
         <v>73565000</v>
       </c>
       <c r="H29" s="4">
@@ -1049,27 +1066,27 @@
         <v>300</v>
       </c>
       <c r="C30" s="6">
-        <f>$G$17+($G$16/(B30*$G$18))</f>
+        <f t="shared" si="4"/>
         <v>34765000</v>
       </c>
       <c r="D30" s="4">
-        <f>B30*$G$18</f>
+        <f t="shared" si="0"/>
         <v>6.0000000000000005E-2</v>
       </c>
       <c r="E30" s="6">
-        <f>C30-$G$23</f>
+        <f t="shared" si="1"/>
         <v>34546250</v>
       </c>
       <c r="F30" s="6">
-        <f>B30*($G$21*(1-$G$15))</f>
+        <f t="shared" si="2"/>
         <v>26250</v>
       </c>
       <c r="G30" s="6">
-        <f>C30-$G$16</f>
+        <f t="shared" si="3"/>
         <v>33565000</v>
       </c>
       <c r="H30" s="4">
-        <f t="shared" ref="H30:H45" si="0">F30/$G$16</f>
+        <f t="shared" ref="H30:H45" si="5">F30/$G$16</f>
         <v>2.1874999999999999E-2</v>
       </c>
     </row>
@@ -1078,27 +1095,27 @@
         <v>500</v>
       </c>
       <c r="C31" s="6">
-        <f>$G$17+($G$16/(B31*$G$18))</f>
+        <f t="shared" si="4"/>
         <v>26765000</v>
       </c>
       <c r="D31" s="4">
-        <f>B31*$G$18</f>
+        <f t="shared" si="0"/>
         <v>0.1</v>
       </c>
       <c r="E31" s="6">
-        <f>C31-$G$23</f>
+        <f t="shared" si="1"/>
         <v>26546250</v>
       </c>
       <c r="F31" s="6">
-        <f>B31*($G$21*(1-$G$15))</f>
+        <f t="shared" si="2"/>
         <v>43750</v>
       </c>
       <c r="G31" s="6">
-        <f>C31-$G$16</f>
+        <f t="shared" si="3"/>
         <v>25565000</v>
       </c>
       <c r="H31" s="4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="5"/>
         <v>3.6458333333333336E-2</v>
       </c>
     </row>
@@ -1107,27 +1124,27 @@
         <v>700</v>
       </c>
       <c r="C32" s="6">
-        <f>$G$17+($G$16/(B32*$G$18))</f>
+        <f t="shared" si="4"/>
         <v>23336428.571428571</v>
       </c>
       <c r="D32" s="4">
-        <f>B32*$G$18</f>
+        <f t="shared" si="0"/>
         <v>0.14000000000000001</v>
       </c>
       <c r="E32" s="6">
-        <f>C32-$G$23</f>
+        <f t="shared" si="1"/>
         <v>23117678.571428571</v>
       </c>
       <c r="F32" s="6">
-        <f>B32*($G$21*(1-$G$15))</f>
+        <f t="shared" si="2"/>
         <v>61250</v>
       </c>
       <c r="G32" s="6">
-        <f>C32-$G$16</f>
+        <f t="shared" si="3"/>
         <v>22136428.571428571</v>
       </c>
       <c r="H32" s="4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="5"/>
         <v>5.1041666666666666E-2</v>
       </c>
     </row>
@@ -1136,27 +1153,27 @@
         <v>1000</v>
       </c>
       <c r="C33" s="6">
-        <f>$G$17+($G$16/(B33*$G$18))</f>
+        <f t="shared" si="4"/>
         <v>20765000</v>
       </c>
       <c r="D33" s="4">
-        <f>B33*$G$18</f>
+        <f t="shared" si="0"/>
         <v>0.2</v>
       </c>
       <c r="E33" s="6">
-        <f>C33-$G$23</f>
+        <f t="shared" si="1"/>
         <v>20546250</v>
       </c>
       <c r="F33" s="6">
-        <f>B33*($G$21*(1-$G$15))</f>
+        <f t="shared" si="2"/>
         <v>87500</v>
       </c>
       <c r="G33" s="6">
-        <f>C33-$G$16</f>
+        <f t="shared" si="3"/>
         <v>19565000</v>
       </c>
       <c r="H33" s="4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="5"/>
         <v>7.2916666666666671E-2</v>
       </c>
     </row>
@@ -1165,27 +1182,27 @@
         <v>1500</v>
       </c>
       <c r="C34" s="6">
-        <f>$G$17+($G$16/(B34*$G$18))</f>
+        <f t="shared" si="4"/>
         <v>18765000</v>
       </c>
       <c r="D34" s="4">
-        <f>B34*$G$18</f>
+        <f t="shared" si="0"/>
         <v>0.3</v>
       </c>
       <c r="E34" s="6">
-        <f>C34-$G$23</f>
+        <f t="shared" si="1"/>
         <v>18546250</v>
       </c>
       <c r="F34" s="6">
-        <f>B34*($G$21*(1-$G$15))</f>
+        <f t="shared" si="2"/>
         <v>131250</v>
       </c>
       <c r="G34" s="6">
-        <f>C34-$G$16</f>
+        <f t="shared" si="3"/>
         <v>17565000</v>
       </c>
       <c r="H34" s="4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="5"/>
         <v>0.109375</v>
       </c>
     </row>
@@ -1194,27 +1211,27 @@
         <v>2000</v>
       </c>
       <c r="C35" s="6">
-        <f>$G$17+($G$16/(B35*$G$18))</f>
+        <f t="shared" si="4"/>
         <v>17765000</v>
       </c>
       <c r="D35" s="4">
-        <f>B35*$G$18</f>
+        <f t="shared" si="0"/>
         <v>0.4</v>
       </c>
       <c r="E35" s="6">
-        <f>C35-$G$23</f>
+        <f t="shared" si="1"/>
         <v>17546250</v>
       </c>
       <c r="F35" s="6">
-        <f>B35*($G$21*(1-$G$15))</f>
+        <f t="shared" si="2"/>
         <v>175000</v>
       </c>
       <c r="G35" s="6">
-        <f>C35-$G$16</f>
+        <f t="shared" si="3"/>
         <v>16565000</v>
       </c>
       <c r="H35" s="4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="5"/>
         <v>0.14583333333333334</v>
       </c>
     </row>
@@ -1223,27 +1240,27 @@
         <v>2500</v>
       </c>
       <c r="C36" s="6">
-        <f>$G$17+($G$16/(B36*$G$18))</f>
+        <f t="shared" si="4"/>
         <v>17165000</v>
       </c>
       <c r="D36" s="4">
-        <f>B36*$G$18</f>
+        <f t="shared" si="0"/>
         <v>0.5</v>
       </c>
       <c r="E36" s="6">
-        <f>C36-$G$23</f>
+        <f t="shared" si="1"/>
         <v>16946250</v>
       </c>
       <c r="F36" s="6">
-        <f>B36*($G$21*(1-$G$15))</f>
+        <f t="shared" si="2"/>
         <v>218750</v>
       </c>
       <c r="G36" s="6">
-        <f>C36-$G$16</f>
+        <f t="shared" si="3"/>
         <v>15965000</v>
       </c>
       <c r="H36" s="4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="5"/>
         <v>0.18229166666666666</v>
       </c>
     </row>
@@ -1252,27 +1269,27 @@
         <v>3000</v>
       </c>
       <c r="C37" s="6">
-        <f>$G$17+($G$16/(B37*$G$18))</f>
+        <f t="shared" si="4"/>
         <v>16765000</v>
       </c>
       <c r="D37" s="4">
-        <f>B37*$G$18</f>
+        <f t="shared" si="0"/>
         <v>0.6</v>
       </c>
       <c r="E37" s="6">
-        <f>C37-$G$23</f>
+        <f t="shared" si="1"/>
         <v>16546250</v>
       </c>
       <c r="F37" s="6">
-        <f>B37*($G$21*(1-$G$15))</f>
+        <f t="shared" si="2"/>
         <v>262500</v>
       </c>
       <c r="G37" s="6">
-        <f>C37-$G$16</f>
+        <f t="shared" si="3"/>
         <v>15565000</v>
       </c>
       <c r="H37" s="4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="5"/>
         <v>0.21875</v>
       </c>
     </row>
@@ -1281,27 +1298,27 @@
         <v>3500</v>
       </c>
       <c r="C38" s="6">
-        <f>$G$17+($G$16/(B38*$G$18))</f>
+        <f t="shared" si="4"/>
         <v>16479285.714285715</v>
       </c>
       <c r="D38" s="4">
-        <f>B38*$G$18</f>
+        <f t="shared" si="0"/>
         <v>0.70000000000000007</v>
       </c>
       <c r="E38" s="6">
-        <f>C38-$G$23</f>
+        <f t="shared" si="1"/>
         <v>16260535.714285715</v>
       </c>
       <c r="F38" s="6">
-        <f>B38*($G$21*(1-$G$15))</f>
+        <f t="shared" si="2"/>
         <v>306250</v>
       </c>
       <c r="G38" s="6">
-        <f>C38-$G$16</f>
+        <f t="shared" si="3"/>
         <v>15279285.714285715</v>
       </c>
       <c r="H38" s="4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="5"/>
         <v>0.25520833333333331</v>
       </c>
     </row>
@@ -1310,27 +1327,27 @@
         <v>4000</v>
       </c>
       <c r="C39" s="6">
-        <f>$G$17+($G$16/(B39*$G$18))</f>
+        <f t="shared" si="4"/>
         <v>16265000</v>
       </c>
       <c r="D39" s="4">
-        <f>B39*$G$18</f>
+        <f t="shared" si="0"/>
         <v>0.8</v>
       </c>
       <c r="E39" s="6">
-        <f>C39-$G$23</f>
+        <f t="shared" si="1"/>
         <v>16046250</v>
       </c>
       <c r="F39" s="6">
-        <f>B39*($G$21*(1-$G$15))</f>
+        <f t="shared" si="2"/>
         <v>350000</v>
       </c>
       <c r="G39" s="6">
-        <f>C39-$G$16</f>
+        <f t="shared" si="3"/>
         <v>15065000</v>
       </c>
       <c r="H39" s="4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="5"/>
         <v>0.29166666666666669</v>
       </c>
     </row>
@@ -1339,27 +1356,27 @@
         <v>4500</v>
       </c>
       <c r="C40" s="6">
-        <f>$G$17+($G$16/(B40*$G$18))</f>
+        <f t="shared" si="4"/>
         <v>16098333.333333334</v>
       </c>
       <c r="D40" s="4">
-        <f>B40*$G$18</f>
+        <f t="shared" si="0"/>
         <v>0.9</v>
       </c>
       <c r="E40" s="6">
-        <f>C40-$G$23</f>
+        <f t="shared" si="1"/>
         <v>15879583.333333334</v>
       </c>
       <c r="F40" s="6">
-        <f>B40*($G$21*(1-$G$15))</f>
+        <f t="shared" si="2"/>
         <v>393750</v>
       </c>
       <c r="G40" s="6">
-        <f>C40-$G$16</f>
+        <f t="shared" si="3"/>
         <v>14898333.333333334</v>
       </c>
       <c r="H40" s="4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="5"/>
         <v>0.328125</v>
       </c>
     </row>
@@ -1368,27 +1385,27 @@
         <v>5000</v>
       </c>
       <c r="C41" s="6">
-        <f>$G$17+($G$16/(B41*$G$18))</f>
+        <f t="shared" si="4"/>
         <v>15965000</v>
       </c>
       <c r="D41" s="4">
-        <f>B41*$G$18</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="E41" s="6">
-        <f>C41-$G$23</f>
+        <f t="shared" si="1"/>
         <v>15746250</v>
       </c>
       <c r="F41" s="6">
-        <f>B41*($G$21*(1-$G$15))</f>
+        <f t="shared" si="2"/>
         <v>437500</v>
       </c>
       <c r="G41" s="6">
-        <f>C41-$G$16</f>
+        <f t="shared" si="3"/>
         <v>14765000</v>
       </c>
       <c r="H41" s="4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="5"/>
         <v>0.36458333333333331</v>
       </c>
     </row>
@@ -1397,27 +1414,27 @@
         <v>10000</v>
       </c>
       <c r="C42" s="6">
-        <f>$G$17+($G$16/(B42*$G$18))</f>
+        <f t="shared" si="4"/>
         <v>15365000</v>
       </c>
       <c r="D42" s="4">
-        <f>B42*$G$18</f>
+        <f t="shared" si="0"/>
         <v>2</v>
       </c>
       <c r="E42" s="6">
-        <f>C42-$G$23</f>
+        <f t="shared" si="1"/>
         <v>15146250</v>
       </c>
       <c r="F42" s="6">
-        <f>B42*($G$21*(1-$G$15))</f>
+        <f t="shared" si="2"/>
         <v>875000</v>
       </c>
       <c r="G42" s="6">
-        <f>C42-$G$16</f>
+        <f t="shared" si="3"/>
         <v>14165000</v>
       </c>
       <c r="H42" s="4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="5"/>
         <v>0.72916666666666663</v>
       </c>
     </row>
@@ -1426,27 +1443,27 @@
         <v>15000</v>
       </c>
       <c r="C43" s="6">
-        <f>$G$17+($G$16/(B43*$G$18))</f>
+        <f t="shared" si="4"/>
         <v>15165000</v>
       </c>
       <c r="D43" s="4">
-        <f>B43*$G$18</f>
+        <f t="shared" si="0"/>
         <v>3</v>
       </c>
       <c r="E43" s="6">
-        <f>C43-$G$23</f>
+        <f t="shared" si="1"/>
         <v>14946250</v>
       </c>
       <c r="F43" s="6">
-        <f>B43*($G$21*(1-$G$15))</f>
+        <f t="shared" si="2"/>
         <v>1312500</v>
       </c>
       <c r="G43" s="6">
-        <f>C43-$G$16</f>
+        <f t="shared" si="3"/>
         <v>13965000</v>
       </c>
       <c r="H43" s="4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="5"/>
         <v>1.09375</v>
       </c>
     </row>
@@ -1455,27 +1472,27 @@
         <v>20000</v>
       </c>
       <c r="C44" s="6">
-        <f>$G$17+($G$16/(B44*$G$18))</f>
+        <f t="shared" si="4"/>
         <v>15065000</v>
       </c>
       <c r="D44" s="4">
-        <f>B44*$G$18</f>
+        <f t="shared" si="0"/>
         <v>4</v>
       </c>
       <c r="E44" s="6">
-        <f>C44-$G$23</f>
+        <f t="shared" si="1"/>
         <v>14846250</v>
       </c>
       <c r="F44" s="6">
-        <f>B44*($G$21*(1-$G$15))</f>
+        <f t="shared" si="2"/>
         <v>1750000</v>
       </c>
       <c r="G44" s="6">
-        <f>C44-$G$16</f>
+        <f t="shared" si="3"/>
         <v>13865000</v>
       </c>
       <c r="H44" s="4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="5"/>
         <v>1.4583333333333333</v>
       </c>
     </row>
@@ -1484,34 +1501,32 @@
         <v>25000</v>
       </c>
       <c r="C45" s="6">
-        <f>$G$17+($G$16/(B45*$G$18))</f>
+        <f t="shared" si="4"/>
         <v>15005000</v>
       </c>
       <c r="D45" s="4">
-        <f>B45*$G$18</f>
+        <f t="shared" si="0"/>
         <v>5</v>
       </c>
       <c r="E45" s="6">
-        <f>C45-$G$23</f>
+        <f t="shared" si="1"/>
         <v>14786250</v>
       </c>
       <c r="F45" s="6">
-        <f>B45*($G$21*(1-$G$15))</f>
+        <f t="shared" si="2"/>
         <v>2187500</v>
       </c>
       <c r="G45" s="6">
-        <f>C45-$G$16</f>
+        <f t="shared" si="3"/>
         <v>13805000</v>
       </c>
       <c r="H45" s="4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="5"/>
         <v>1.8229166666666667</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="20">
-    <mergeCell ref="E15:F15"/>
-    <mergeCell ref="G15:H15"/>
     <mergeCell ref="B25:H26"/>
     <mergeCell ref="E20:F20"/>
     <mergeCell ref="G20:H20"/>
@@ -1519,9 +1534,6 @@
     <mergeCell ref="G22:H22"/>
     <mergeCell ref="E23:F23"/>
     <mergeCell ref="G23:H23"/>
-    <mergeCell ref="G18:H18"/>
-    <mergeCell ref="G17:H17"/>
-    <mergeCell ref="G16:H16"/>
     <mergeCell ref="B11:H13"/>
     <mergeCell ref="E21:F21"/>
     <mergeCell ref="E19:F19"/>
@@ -1530,10 +1542,19 @@
     <mergeCell ref="E16:F16"/>
     <mergeCell ref="G21:H21"/>
     <mergeCell ref="G19:H19"/>
+    <mergeCell ref="E15:F15"/>
+    <mergeCell ref="G15:H15"/>
+    <mergeCell ref="G18:H18"/>
+    <mergeCell ref="G17:H17"/>
+    <mergeCell ref="G16:H16"/>
   </mergeCells>
+  <hyperlinks>
+    <hyperlink ref="C20" r:id="rId1" xr:uid="{B0BB3CFF-4EF8-4213-A811-9067C58A1058}"/>
+    <hyperlink ref="C21" r:id="rId2" xr:uid="{5DD29EC0-95D4-4200-ABC6-1A5BD540B1D4}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId1"/>
-  <drawing r:id="rId2"/>
+  <pageSetup orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId3"/>
+  <drawing r:id="rId4"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
@@ -1551,10 +1572,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{705FF274-E9A4-46A8-8F07-0B043A01F8C8}">
-  <dimension ref="B4:I14"/>
+  <dimension ref="B4:I17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+      <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -1564,157 +1585,163 @@
   </cols>
   <sheetData>
     <row r="4" spans="2:9" x14ac:dyDescent="0.45">
-      <c r="B4" s="23" t="s">
-        <v>42</v>
+      <c r="B4" s="13" t="s">
+        <v>39</v>
       </c>
       <c r="C4" s="3">
         <v>14589176</v>
       </c>
-      <c r="E4" s="12" t="s">
-        <v>53</v>
-      </c>
-      <c r="F4" s="12"/>
-      <c r="G4" s="12"/>
-      <c r="H4" s="12"/>
-      <c r="I4" s="12"/>
+      <c r="E4" s="25" t="s">
+        <v>50</v>
+      </c>
+      <c r="F4" s="25"/>
+      <c r="G4" s="25"/>
+      <c r="H4" s="25"/>
+      <c r="I4" s="25"/>
     </row>
     <row r="5" spans="2:9" x14ac:dyDescent="0.45">
-      <c r="B5" s="23" t="s">
-        <v>43</v>
+      <c r="B5" s="13" t="s">
+        <v>40</v>
       </c>
       <c r="C5" s="3">
         <v>14765000</v>
       </c>
-      <c r="E5" s="12"/>
-      <c r="F5" s="12"/>
-      <c r="G5" s="12"/>
-      <c r="H5" s="12"/>
-      <c r="I5" s="12"/>
+      <c r="E5" s="25"/>
+      <c r="F5" s="25"/>
+      <c r="G5" s="25"/>
+      <c r="H5" s="25"/>
+      <c r="I5" s="25"/>
     </row>
     <row r="6" spans="2:9" x14ac:dyDescent="0.45">
-      <c r="B6" s="23" t="s">
-        <v>44</v>
+      <c r="B6" s="13" t="s">
+        <v>41</v>
       </c>
       <c r="C6">
         <f>C5-C4</f>
         <v>175824</v>
       </c>
-      <c r="E6" s="12"/>
-      <c r="F6" s="12"/>
-      <c r="G6" s="12"/>
-      <c r="H6" s="12"/>
-      <c r="I6" s="12"/>
+      <c r="E6" s="25"/>
+      <c r="F6" s="25"/>
+      <c r="G6" s="25"/>
+      <c r="H6" s="25"/>
+      <c r="I6" s="25"/>
     </row>
     <row r="7" spans="2:9" x14ac:dyDescent="0.45">
-      <c r="B7" s="23" t="s">
-        <v>45</v>
+      <c r="B7" s="13" t="s">
+        <v>42</v>
       </c>
       <c r="C7">
         <v>2</v>
       </c>
-      <c r="E7" s="12"/>
-      <c r="F7" s="12"/>
-      <c r="G7" s="12"/>
-      <c r="H7" s="12"/>
-      <c r="I7" s="12"/>
+      <c r="E7" s="25"/>
+      <c r="F7" s="25"/>
+      <c r="G7" s="25"/>
+      <c r="H7" s="25"/>
+      <c r="I7" s="25"/>
     </row>
     <row r="8" spans="2:9" x14ac:dyDescent="0.45">
-      <c r="B8" s="23" t="s">
-        <v>46</v>
+      <c r="B8" s="13" t="s">
+        <v>43</v>
       </c>
       <c r="C8">
         <f>C6*2</f>
         <v>351648</v>
       </c>
-      <c r="E8" s="12"/>
-      <c r="F8" s="12"/>
-      <c r="G8" s="12"/>
-      <c r="H8" s="12"/>
-      <c r="I8" s="12"/>
+      <c r="E8" s="25"/>
+      <c r="F8" s="25"/>
+      <c r="G8" s="25"/>
+      <c r="H8" s="25"/>
+      <c r="I8" s="25"/>
     </row>
     <row r="9" spans="2:9" x14ac:dyDescent="0.45">
-      <c r="B9" s="23" t="s">
-        <v>47</v>
+      <c r="B9" s="13" t="s">
+        <v>44</v>
       </c>
       <c r="C9">
         <f>C8/60</f>
         <v>5860.8</v>
       </c>
-      <c r="E9" s="12"/>
-      <c r="F9" s="12"/>
-      <c r="G9" s="12"/>
-      <c r="H9" s="12"/>
-      <c r="I9" s="12"/>
+      <c r="E9" s="25"/>
+      <c r="F9" s="25"/>
+      <c r="G9" s="25"/>
+      <c r="H9" s="25"/>
+      <c r="I9" s="25"/>
     </row>
     <row r="10" spans="2:9" x14ac:dyDescent="0.45">
-      <c r="B10" s="23" t="s">
-        <v>48</v>
+      <c r="B10" s="13" t="s">
+        <v>45</v>
       </c>
       <c r="C10">
         <f>C9/60</f>
         <v>97.68</v>
       </c>
-      <c r="E10" s="12"/>
-      <c r="F10" s="12"/>
-      <c r="G10" s="12"/>
-      <c r="H10" s="12"/>
-      <c r="I10" s="12"/>
+      <c r="E10" s="25"/>
+      <c r="F10" s="25"/>
+      <c r="G10" s="25"/>
+      <c r="H10" s="25"/>
+      <c r="I10" s="25"/>
     </row>
     <row r="11" spans="2:9" x14ac:dyDescent="0.45">
-      <c r="B11" s="23" t="s">
-        <v>49</v>
+      <c r="B11" s="13" t="s">
+        <v>46</v>
       </c>
       <c r="C11">
         <f>C10/24</f>
         <v>4.07</v>
       </c>
-      <c r="E11" s="12"/>
-      <c r="F11" s="12"/>
-      <c r="G11" s="12"/>
-      <c r="H11" s="12"/>
-      <c r="I11" s="12"/>
+      <c r="E11" s="25"/>
+      <c r="F11" s="25"/>
+      <c r="G11" s="25"/>
+      <c r="H11" s="25"/>
+      <c r="I11" s="25"/>
     </row>
     <row r="12" spans="2:9" x14ac:dyDescent="0.45">
-      <c r="B12" s="23" t="s">
-        <v>50</v>
+      <c r="B12" s="13" t="s">
+        <v>47</v>
       </c>
       <c r="C12">
         <f>C11/7</f>
         <v>0.58142857142857152</v>
       </c>
-      <c r="E12" s="12"/>
-      <c r="F12" s="12"/>
-      <c r="G12" s="12"/>
-      <c r="H12" s="12"/>
-      <c r="I12" s="12"/>
+      <c r="E12" s="25"/>
+      <c r="F12" s="25"/>
+      <c r="G12" s="25"/>
+      <c r="H12" s="25"/>
+      <c r="I12" s="25"/>
     </row>
     <row r="13" spans="2:9" x14ac:dyDescent="0.45">
-      <c r="B13" s="23" t="s">
-        <v>51</v>
+      <c r="B13" s="13" t="s">
+        <v>48</v>
       </c>
       <c r="C13">
         <f>C12/4</f>
         <v>0.14535714285714288</v>
       </c>
-      <c r="E13" s="12"/>
-      <c r="F13" s="12"/>
-      <c r="G13" s="12"/>
-      <c r="H13" s="12"/>
-      <c r="I13" s="12"/>
+      <c r="E13" s="25"/>
+      <c r="F13" s="25"/>
+      <c r="G13" s="25"/>
+      <c r="H13" s="25"/>
+      <c r="I13" s="25"/>
     </row>
     <row r="14" spans="2:9" x14ac:dyDescent="0.45">
-      <c r="B14" s="23" t="s">
-        <v>52</v>
+      <c r="B14" s="13" t="s">
+        <v>49</v>
       </c>
       <c r="C14">
         <f>C13/12</f>
         <v>1.2113095238095241E-2</v>
       </c>
-      <c r="E14" s="12"/>
-      <c r="F14" s="12"/>
-      <c r="G14" s="12"/>
-      <c r="H14" s="12"/>
-      <c r="I14" s="12"/>
+      <c r="E14" s="25"/>
+      <c r="F14" s="25"/>
+      <c r="G14" s="25"/>
+      <c r="H14" s="25"/>
+      <c r="I14" s="25"/>
+    </row>
+    <row r="17" spans="3:3" x14ac:dyDescent="0.45">
+      <c r="C17" s="26">
+        <f ca="1">NOW()+C11</f>
+        <v>44375.88591921296</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -1744,36 +1771,36 @@
   <sheetData>
     <row r="2" spans="2:7" x14ac:dyDescent="0.45">
       <c r="B2" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="E2" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="C2" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="D2" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="E2" s="4" t="s">
-        <v>34</v>
-      </c>
       <c r="F2" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="G2" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="G2" s="4" t="s">
-        <v>36</v>
-      </c>
     </row>
     <row r="3" spans="2:7" x14ac:dyDescent="0.45">
-      <c r="B3" s="13" t="s">
-        <v>26</v>
-      </c>
-      <c r="C3" s="13" t="s">
-        <v>38</v>
+      <c r="B3" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="C3" s="8" t="s">
+        <v>35</v>
       </c>
       <c r="D3" s="4">
         <v>50</v>
       </c>
-      <c r="E3" s="13" t="s">
-        <v>35</v>
+      <c r="E3" s="8" t="s">
+        <v>32</v>
       </c>
       <c r="F3" s="4">
         <v>51</v>
@@ -1783,16 +1810,16 @@
       </c>
     </row>
     <row r="4" spans="2:7" x14ac:dyDescent="0.45">
-      <c r="B4" s="13" t="s">
-        <v>27</v>
-      </c>
-      <c r="C4" s="13" t="s">
-        <v>39</v>
+      <c r="B4" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="C4" s="8" t="s">
+        <v>36</v>
       </c>
       <c r="D4" s="4">
         <v>0</v>
       </c>
-      <c r="E4" s="13" t="s">
+      <c r="E4" s="8" t="s">
         <v>0</v>
       </c>
       <c r="F4" s="4">
@@ -1803,16 +1830,16 @@
       </c>
     </row>
     <row r="5" spans="2:7" x14ac:dyDescent="0.45">
-      <c r="B5" s="13" t="s">
-        <v>28</v>
-      </c>
-      <c r="C5" s="13" t="s">
-        <v>40</v>
+      <c r="B5" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="C5" s="8" t="s">
+        <v>37</v>
       </c>
       <c r="D5" s="4">
         <v>10</v>
       </c>
-      <c r="E5" s="13" t="s">
+      <c r="E5" s="8" t="s">
         <v>0</v>
       </c>
       <c r="F5" s="4">
@@ -1823,16 +1850,16 @@
       </c>
     </row>
     <row r="6" spans="2:7" x14ac:dyDescent="0.45">
-      <c r="B6" s="13" t="s">
-        <v>29</v>
-      </c>
-      <c r="C6" s="13" t="s">
-        <v>54</v>
+      <c r="B6" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="C6" s="8" t="s">
+        <v>51</v>
       </c>
       <c r="D6" s="4">
         <v>50</v>
       </c>
-      <c r="E6" s="13" t="s">
+      <c r="E6" s="8" t="s">
         <v>0</v>
       </c>
       <c r="F6" s="4">
@@ -1843,16 +1870,16 @@
       </c>
     </row>
     <row r="7" spans="2:7" x14ac:dyDescent="0.45">
-      <c r="B7" s="13" t="s">
-        <v>30</v>
-      </c>
-      <c r="C7" s="13" t="s">
-        <v>41</v>
+      <c r="B7" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="C7" s="8" t="s">
+        <v>38</v>
       </c>
       <c r="D7" s="4">
         <v>100</v>
       </c>
-      <c r="E7" s="13" t="s">
+      <c r="E7" s="8" t="s">
         <v>0</v>
       </c>
       <c r="F7" s="4">

</xml_diff>